<commit_message>
Updated to match submission
Changes formatting of quantities to be "number" instead of "text" in Microsoft Excel
</commit_message>
<xml_diff>
--- a/web/public/documents/A7 - Bill of Materials.xlsx
+++ b/web/public/documents/A7 - Bill of Materials.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moorm\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDA8D82-BEA5-4095-9D3F-A1132164A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="MPTXz4yAdzGVxVK3Qv6r8GyaEL/hzI6koLGMi8P0b8I="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="121">
   <si>
     <t>ECE477 Bill of Materials v1.0</t>
   </si>
@@ -45,9 +54,6 @@
     <t>Qty:</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -102,9 +108,6 @@
     <t>SSD1309</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Teyleten Robot</t>
   </si>
   <si>
@@ -183,9 +186,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>ECE Shop</t>
   </si>
   <si>
@@ -228,9 +228,6 @@
     <t>9-146280-0-08</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Daughterboard</t>
   </si>
   <si>
-    <t>128</t>
-  </si>
-  <si>
     <t>Digital Hall Effect Sensors</t>
   </si>
   <si>
@@ -294,9 +288,6 @@
     <t>9-103325-0-08</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>A32702-08-ND</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>ED-DP_L10_F-F_120pcs</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>EDGELEC</t>
   </si>
   <si>
@@ -379,9 +367,6 @@
   </si>
   <si>
     <t>Wood Panels</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
   <si>
     <t>N/A</t>
@@ -408,33 +393,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -445,29 +435,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="9">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -482,8 +483,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -493,107 +496,100 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -783,1002 +779,1004 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L1010"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="67.14"/>
-    <col customWidth="1" min="2" max="2" width="21.14"/>
-    <col customWidth="1" min="3" max="3" width="5.14"/>
-    <col customWidth="1" min="4" max="4" width="21.57"/>
-    <col customWidth="1" min="5" max="5" width="12.71"/>
-    <col customWidth="1" min="6" max="6" width="20.57"/>
-    <col customWidth="1" min="7" max="7" width="20.43"/>
-    <col customWidth="1" min="8" max="8" width="19.86"/>
-    <col customWidth="1" min="9" max="9" width="27.0"/>
-    <col customWidth="1" min="10" max="10" width="4.29"/>
-    <col customWidth="1" min="11" max="26" width="8.71"/>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="21">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="21">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="21">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="21">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="21">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="21">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="21">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="21">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="21">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="21">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="21">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="21">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="I25" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="21">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="21">
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="21">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="21">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="21">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="I30" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="11"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
+      <c r="B33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="21">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A36" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="21">
+        <v>1</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="21">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="21">
         <v>8</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J29" s="10"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I36" s="11" t="s">
+      <c r="D38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="G38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="19" t="s">
+      <c r="I38" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="B39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="C39" s="21">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I37" s="11" t="s">
+      <c r="E39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="G39" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2743,11 +2741,21 @@
     <row r="1010" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I21:J21"/>
@@ -2759,25 +2767,13 @@
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>